<commit_message>
Finalizei a aula 4
</commit_message>
<xml_diff>
--- a/Excel VBA/Aula 4 - Criando Gráficos/Produtos.xlsx
+++ b/Excel VBA/Aula 4 - Criando Gráficos/Produtos.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 3 - Cálculos Básicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\bruno\Documents\GitHub\Alura\Excel VBA\Aula 4 - Criando Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB945D6-847A-4F56-AD5D-17FEA97F4FC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0A005-D987-4BB5-8A66-9AD62E3EE416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{F429CDF2-33A2-4A6E-9034-27FA88637C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos Adultos" sheetId="3" r:id="rId1"/>
     <sheet name="Produtos Infantis" sheetId="1" r:id="rId2"/>
+    <sheet name="Gráficos" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -373,13 +374,13 @@
     <xf numFmtId="9" fontId="6" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="44" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -398,6 +399,2225 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.3013114183629269E-2"/>
+          <c:y val="7.8341917448794679E-2"/>
+          <c:w val="0.91250128835754063"/>
+          <c:h val="0.56219497672908614"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Produtos Infantis'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Valor Total </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Produtos Infantis'!$A$3:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Produtos Infantis'!$F$3:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>153.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>269.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>427.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>269.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>179.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>269.70000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C646-45CB-BB65-B89EFB5B65F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1297168111"/>
+        <c:axId val="1297185999"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1297168111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1297185999"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1297185999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1297168111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Composição do Estoque</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="50"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.5954418817671682E-2"/>
+          <c:y val="8.6209253255107823E-2"/>
+          <c:w val="0.6097583255505441"/>
+          <c:h val="0.8615031650455458"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Produtos Infantis'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantidades</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-C28D-4486-8E06-F12558B3A0A5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Produtos Infantis'!$A$3:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tênis Infantil Vermelho</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Tênis Infantil Azul</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Tênis Infantil Rosa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Produtos Infantis'!$E$3:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-C28D-4486-8E06-F12558B3A0A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="264">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91E7FFBE-DA3B-4DCB-AB7F-A7922840CFC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20DEBA9B-0403-4474-B1E3-EA31EE4423CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6CF0F7-701F-4AD3-A160-66200CB65652}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" activeCellId="1" sqref="A2:A11 E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +3146,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="11">
-        <f>C4*E4</f>
+        <f t="shared" ref="F4:F11" si="1">C4*E4</f>
         <v>269.70000000000005</v>
       </c>
     </row>
@@ -948,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="11">
-        <f>C5*E5</f>
+        <f t="shared" si="1"/>
         <v>89.9</v>
       </c>
     </row>
@@ -970,7 +3190,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="11">
-        <f>C6*E6</f>
+        <f t="shared" si="1"/>
         <v>427.5</v>
       </c>
     </row>
@@ -992,7 +3212,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="11">
-        <f>C7*E7</f>
+        <f t="shared" si="1"/>
         <v>269.70000000000005</v>
       </c>
     </row>
@@ -1014,7 +3234,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="11">
-        <f>C8*E8</f>
+        <f t="shared" si="1"/>
         <v>269.70000000000005</v>
       </c>
     </row>
@@ -1036,7 +3256,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="11">
-        <f>C9*E9</f>
+        <f t="shared" si="1"/>
         <v>85.5</v>
       </c>
     </row>
@@ -1058,7 +3278,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="11">
-        <f>C10*E10</f>
+        <f t="shared" si="1"/>
         <v>179.8</v>
       </c>
     </row>
@@ -1080,7 +3300,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="11">
-        <f>C11*E11</f>
+        <f t="shared" si="1"/>
         <v>269.70000000000005</v>
       </c>
     </row>
@@ -1111,9 +3331,9 @@
       <c r="C13" s="20">
         <v>0.1</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1125,4 +3345,19 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DC4B28-A0EC-435B-9AD3-BBF63385D2CE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>